<commit_message>
LTC3: Modified LTC schematic.
Replaced ST Micro 74V1G08CTR single, two-input AND gate with a TI
SN74AHC1G08 (also a single, two-input AND gate).  This required a
footprint change, so it will impact the PCB layout.
</commit_message>
<xml_diff>
--- a/ltc3/bom/ltc/LTC3.xlsx
+++ b/ltc3/bom/ltc/LTC3.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1924" uniqueCount="459">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1924" uniqueCount="458">
   <si>
     <t xml:space="preserve">Refs</t>
   </si>
@@ -1297,19 +1297,16 @@
     <t xml:space="preserve">U403</t>
   </si>
   <si>
-    <t xml:space="preserve">74V1G08</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OBSOLETE PART!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STMicro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">74V1G08CTR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LTC3:SOT323-5L</t>
+    <t xml:space="preserve">SN74AHC1G08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SN74AHC1G08DCKR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 input AND gate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TO_SOT_Packages_SMD:SC-70-5</t>
   </si>
   <si>
     <t xml:space="preserve">U404</t>
@@ -1454,14 +1451,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF99"/>
-        <bgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFFF9999"/>
+        <bgColor rgb="FFFF8080"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF9999"/>
-        <bgColor rgb="FFFF8080"/>
+        <fgColor rgb="FFFFFF99"/>
+        <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -1506,7 +1503,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1527,15 +1524,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1618,22 +1611,22 @@
   </sheetPr>
   <dimension ref="A1:I65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A58" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D73" activeCellId="0" sqref="D73"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A24" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B193" activeCellId="0" sqref="B193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.9948979591837"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.984693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.6428571428571"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.8622448979592"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="29.2908163265306"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="54.6734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.5867346938776"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.2397959183673"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.4591836734694"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="28.8877551020408"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="54.1326530612245"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="20.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2361,7 +2354,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="26" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
         <v>64</v>
       </c>
@@ -2390,7 +2383,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="27" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
         <v>66</v>
       </c>
@@ -2419,7 +2412,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="28" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
         <v>67</v>
       </c>
@@ -2448,7 +2441,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="29" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
         <v>68</v>
       </c>
@@ -2477,7 +2470,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
         <v>69</v>
       </c>
@@ -2506,7 +2499,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="31" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
         <v>74</v>
       </c>
@@ -2535,7 +2528,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="32" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
         <v>75</v>
       </c>
@@ -2564,7 +2557,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="33" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
         <v>76</v>
       </c>
@@ -2593,7 +2586,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="34" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
         <v>77</v>
       </c>
@@ -2622,7 +2615,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="35" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
         <v>78</v>
       </c>
@@ -2649,7 +2642,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="36" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
         <v>85</v>
       </c>
@@ -2678,7 +2671,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="37" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="s">
         <v>86</v>
       </c>
@@ -2705,7 +2698,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="38" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
         <v>88</v>
       </c>
@@ -2734,7 +2727,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="39" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="s">
         <v>94</v>
       </c>
@@ -2763,7 +2756,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="40" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="s">
         <v>100</v>
       </c>
@@ -2792,7 +2785,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="41" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="s">
         <v>102</v>
       </c>
@@ -2821,7 +2814,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="42" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="s">
         <v>107</v>
       </c>
@@ -2850,7 +2843,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="43" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="s">
         <v>112</v>
       </c>
@@ -2863,10 +2856,10 @@
       <c r="D43" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="E43" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F43" s="4" t="s">
+      <c r="E43" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F43" s="5" t="s">
         <v>12</v>
       </c>
       <c r="G43" s="2" t="s">
@@ -2879,7 +2872,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="44" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="s">
         <v>116</v>
       </c>
@@ -2908,7 +2901,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="45" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="2" t="s">
         <v>119</v>
       </c>
@@ -2921,10 +2914,10 @@
       <c r="D45" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="E45" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F45" s="4" t="s">
+      <c r="E45" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F45" s="5" t="s">
         <v>12</v>
       </c>
       <c r="G45" s="2" t="s">
@@ -2937,7 +2930,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="46" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="2" t="s">
         <v>123</v>
       </c>
@@ -2950,10 +2943,10 @@
       <c r="D46" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="E46" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F46" s="4" t="s">
+      <c r="E46" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F46" s="5" t="s">
         <v>12</v>
       </c>
       <c r="G46" s="2" t="s">
@@ -2966,7 +2959,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="47" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="s">
         <v>124</v>
       </c>
@@ -2979,10 +2972,10 @@
       <c r="D47" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="E47" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F47" s="4" t="s">
+      <c r="E47" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F47" s="5" t="s">
         <v>12</v>
       </c>
       <c r="G47" s="2" t="s">
@@ -2995,7 +2988,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="48" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="2" t="s">
         <v>125</v>
       </c>
@@ -3008,10 +3001,10 @@
       <c r="D48" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="E48" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F48" s="4" t="s">
+      <c r="E48" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F48" s="5" t="s">
         <v>12</v>
       </c>
       <c r="G48" s="2" t="s">
@@ -3024,7 +3017,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="49" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="2" t="s">
         <v>126</v>
       </c>
@@ -3053,7 +3046,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="50" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="2" t="s">
         <v>132</v>
       </c>
@@ -3082,7 +3075,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="51" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="2" t="s">
         <v>133</v>
       </c>
@@ -3111,7 +3104,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="52" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="2" t="s">
         <v>139</v>
       </c>
@@ -3140,7 +3133,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="53" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="2" t="s">
         <v>143</v>
       </c>
@@ -3169,7 +3162,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="54" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="2" t="s">
         <v>144</v>
       </c>
@@ -3198,7 +3191,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="55" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="2" t="s">
         <v>145</v>
       </c>
@@ -3227,670 +3220,670 @@
         <v>16</v>
       </c>
     </row>
-    <row r="56" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="5" t="s">
+    <row r="56" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="B56" s="5" t="s">
+      <c r="B56" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="C56" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D56" s="5" t="s">
+      <c r="C56" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D56" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="E56" s="5" t="s">
+      <c r="E56" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="F56" s="5" t="s">
+      <c r="F56" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="G56" s="5" t="s">
+      <c r="G56" s="2" t="s">
         <v>151</v>
       </c>
       <c r="H56" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="I56" s="5" t="s">
+      <c r="I56" s="2" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="57" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="5" t="s">
+    <row r="57" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="B57" s="5" t="s">
+      <c r="B57" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="C57" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D57" s="5" t="s">
+      <c r="C57" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D57" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="E57" s="6" t="s">
+      <c r="E57" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="F57" s="6" t="s">
+      <c r="F57" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="G57" s="6" t="s">
+      <c r="G57" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="H57" s="6" t="s">
+      <c r="H57" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="I57" s="6" t="s">
+      <c r="I57" s="3" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="58" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="5" t="s">
+    <row r="58" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="B58" s="5" t="s">
+      <c r="B58" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="C58" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D58" s="5" t="s">
+      <c r="C58" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D58" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="E58" s="6" t="s">
+      <c r="E58" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="F58" s="6" t="s">
+      <c r="F58" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="G58" s="6" t="s">
+      <c r="G58" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="H58" s="6" t="s">
+      <c r="H58" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="I58" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="59" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="5" t="s">
+      <c r="I58" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="59" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="B59" s="5" t="s">
+      <c r="B59" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C59" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D59" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E59" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F59" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G59" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H59" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I59" s="6" t="s">
+      <c r="C59" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E59" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F59" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H59" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I59" s="3" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="60" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="5" t="s">
+    <row r="60" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="B60" s="5" t="s">
+      <c r="B60" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C60" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D60" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E60" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F60" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G60" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H60" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I60" s="6" t="s">
+      <c r="C60" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E60" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F60" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H60" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I60" s="3" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="61" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="5" t="s">
+    <row r="61" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="B61" s="5" t="s">
+      <c r="B61" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C61" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D61" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E61" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F61" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G61" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H61" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I61" s="6" t="s">
+      <c r="C61" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E61" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F61" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H61" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I61" s="3" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="62" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="5" t="s">
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="B62" s="5" t="s">
+      <c r="B62" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="C62" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D62" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E62" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F62" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G62" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H62" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I62" s="5" t="s">
+      <c r="C62" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E62" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F62" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G62" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H62" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I62" s="2" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="63" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="5" t="s">
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="B63" s="5" t="s">
+      <c r="B63" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="C63" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D63" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E63" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F63" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G63" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H63" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I63" s="5" t="s">
+      <c r="C63" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E63" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F63" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G63" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H63" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I63" s="2" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="64" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="5" t="s">
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="B64" s="5" t="s">
+      <c r="B64" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="C64" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D64" s="5" t="s">
+      <c r="C64" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D64" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="E64" s="6" t="s">
+      <c r="E64" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="F64" s="6" t="s">
+      <c r="F64" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="G64" s="6" t="s">
+      <c r="G64" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="H64" s="6" t="s">
+      <c r="H64" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="I64" s="6" t="s">
+      <c r="I64" s="3" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="65" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="5" t="s">
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="B65" s="5" t="s">
+      <c r="B65" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="C65" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D65" s="5" t="s">
+      <c r="C65" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D65" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="E65" s="6" t="s">
+      <c r="E65" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="F65" s="6" t="s">
+      <c r="F65" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="G65" s="6" t="s">
+      <c r="G65" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="H65" s="6" t="s">
+      <c r="H65" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="I65" s="6" t="s">
+      <c r="I65" s="3" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="66" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="5" t="s">
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="B66" s="5" t="s">
+      <c r="B66" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="C66" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D66" s="5" t="s">
+      <c r="C66" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D66" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="E66" s="5" t="s">
+      <c r="E66" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="F66" s="5" t="s">
+      <c r="F66" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="G66" s="5" t="s">
+      <c r="G66" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="H66" s="6" t="s">
+      <c r="H66" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="I66" s="5" t="s">
+      <c r="I66" s="2" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="67" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="5" t="s">
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="B67" s="5" t="s">
+      <c r="B67" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="C67" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D67" s="5" t="s">
+      <c r="C67" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D67" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="E67" s="6" t="s">
+      <c r="E67" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="F67" s="6" t="s">
+      <c r="F67" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="G67" s="6" t="s">
+      <c r="G67" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="H67" s="6" t="s">
+      <c r="H67" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="I67" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="68" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="5" t="s">
+      <c r="I67" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="B68" s="5" t="s">
+      <c r="B68" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="C68" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D68" s="5" t="s">
+      <c r="C68" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D68" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="E68" s="5" t="s">
+      <c r="E68" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="F68" s="5" t="s">
+      <c r="F68" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="G68" s="5" t="s">
+      <c r="G68" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="H68" s="6" t="s">
+      <c r="H68" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="I68" s="5" t="s">
+      <c r="I68" s="2" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="69" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="5" t="s">
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="B69" s="5" t="s">
+      <c r="B69" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="C69" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D69" s="5" t="s">
+      <c r="C69" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D69" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="E69" s="5" t="s">
+      <c r="E69" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="F69" s="5" t="s">
+      <c r="F69" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="G69" s="5" t="s">
+      <c r="G69" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="H69" s="6" t="s">
+      <c r="H69" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="I69" s="5" t="s">
+      <c r="I69" s="2" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="70" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="5" t="s">
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="B70" s="5" t="s">
+      <c r="B70" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="C70" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D70" s="5" t="s">
+      <c r="C70" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D70" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="E70" s="6" t="s">
+      <c r="E70" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="F70" s="6" t="s">
+      <c r="F70" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="G70" s="6" t="s">
+      <c r="G70" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="H70" s="6" t="s">
+      <c r="H70" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="I70" s="6" t="s">
+      <c r="I70" s="3" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="71" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="5" t="s">
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="B71" s="5" t="s">
+      <c r="B71" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="C71" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D71" s="5" t="s">
+      <c r="C71" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D71" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="E71" s="5" t="s">
+      <c r="E71" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="F71" s="5" t="s">
+      <c r="F71" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="G71" s="5" t="s">
+      <c r="G71" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="H71" s="6" t="s">
+      <c r="H71" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="I71" s="5" t="s">
+      <c r="I71" s="2" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="72" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="5" t="s">
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="B72" s="5" t="s">
+      <c r="B72" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="C72" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D72" s="5" t="s">
+      <c r="C72" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D72" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="E72" s="6" t="s">
+      <c r="E72" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="F72" s="6" t="s">
+      <c r="F72" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="G72" s="6" t="s">
+      <c r="G72" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="H72" s="6" t="s">
+      <c r="H72" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="I72" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="73" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="5" t="s">
+      <c r="I72" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="B73" s="4" t="s">
+      <c r="B73" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="C73" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D73" s="5" t="s">
+      <c r="C73" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D73" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="E73" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F73" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G73" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H73" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="I73" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="74" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="5" t="s">
+      <c r="E73" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F73" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G73" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H73" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I73" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="B74" s="5" t="s">
+      <c r="B74" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="C74" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D74" s="5" t="s">
+      <c r="C74" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D74" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="E74" s="6" t="s">
+      <c r="E74" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="F74" s="6" t="s">
+      <c r="F74" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="G74" s="6" t="s">
+      <c r="G74" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="H74" s="6" t="s">
+      <c r="H74" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="I74" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="75" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="5" t="s">
+      <c r="I74" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="B75" s="5" t="s">
+      <c r="B75" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="C75" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D75" s="5" t="s">
+      <c r="C75" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D75" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="E75" s="5" t="s">
+      <c r="E75" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="F75" s="5" t="s">
+      <c r="F75" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="G75" s="5" t="s">
+      <c r="G75" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="H75" s="6" t="s">
+      <c r="H75" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="I75" s="5" t="s">
+      <c r="I75" s="2" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="76" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="5" t="s">
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="B76" s="5" t="s">
+      <c r="B76" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="C76" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D76" s="5" t="s">
+      <c r="C76" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D76" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="E76" s="5" t="s">
+      <c r="E76" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="F76" s="5" t="s">
+      <c r="F76" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="G76" s="5" t="s">
+      <c r="G76" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="H76" s="6" t="s">
+      <c r="H76" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="I76" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="77" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="5" t="s">
+      <c r="I76" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="B77" s="5" t="s">
+      <c r="B77" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="C77" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D77" s="5" t="s">
+      <c r="C77" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D77" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="E77" s="5" t="s">
+      <c r="E77" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="F77" s="5" t="s">
+      <c r="F77" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="G77" s="5" t="s">
+      <c r="G77" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="H77" s="6" t="s">
+      <c r="H77" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="I77" s="5" t="s">
+      <c r="I77" s="2" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="78" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="5" t="s">
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="B78" s="5" t="s">
+      <c r="B78" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="C78" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D78" s="5" t="s">
+      <c r="C78" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D78" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="E78" s="5" t="s">
+      <c r="E78" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="F78" s="5" t="s">
+      <c r="F78" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="G78" s="5" t="s">
+      <c r="G78" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="H78" s="6" t="s">
+      <c r="H78" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="I78" s="5" t="s">
+      <c r="I78" s="2" t="s">
         <v>16</v>
       </c>
     </row>
@@ -4126,61 +4119,61 @@
         <v>16</v>
       </c>
     </row>
-    <row r="87" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="5" t="s">
+    <row r="87" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="B87" s="5" t="s">
+      <c r="B87" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="C87" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D87" s="5" t="s">
+      <c r="C87" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D87" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="E87" s="5" t="s">
+      <c r="E87" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="F87" s="5" t="s">
+      <c r="F87" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="G87" s="5" t="s">
+      <c r="G87" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="H87" s="6" t="s">
+      <c r="H87" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="I87" s="5" t="s">
+      <c r="I87" s="2" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="88" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="5" t="s">
+    <row r="88" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="B88" s="5" t="s">
+      <c r="B88" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="C88" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D88" s="5" t="s">
+      <c r="C88" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D88" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="E88" s="5" t="s">
+      <c r="E88" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="F88" s="5" t="s">
+      <c r="F88" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="G88" s="5" t="s">
+      <c r="G88" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="H88" s="6" t="s">
+      <c r="H88" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="I88" s="5" t="s">
+      <c r="I88" s="2" t="s">
         <v>16</v>
       </c>
     </row>
@@ -5112,7 +5105,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="121" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="2" t="s">
         <v>296</v>
       </c>
@@ -5141,7 +5134,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="122" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="2" t="s">
         <v>297</v>
       </c>
@@ -5170,7 +5163,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="123" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="2" t="s">
         <v>300</v>
       </c>
@@ -5199,7 +5192,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="124" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="2" t="s">
         <v>301</v>
       </c>
@@ -5228,7 +5221,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="125" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="2" t="s">
         <v>302</v>
       </c>
@@ -5257,7 +5250,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="126" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="2" t="s">
         <v>303</v>
       </c>
@@ -5286,7 +5279,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="127" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="2" t="s">
         <v>306</v>
       </c>
@@ -5315,7 +5308,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="128" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="2" t="s">
         <v>307</v>
       </c>
@@ -5344,7 +5337,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="129" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="2" t="s">
         <v>308</v>
       </c>
@@ -5373,7 +5366,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="130" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="2" t="s">
         <v>309</v>
       </c>
@@ -5402,7 +5395,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="131" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="2" t="s">
         <v>312</v>
       </c>
@@ -5431,7 +5424,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="132" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="2" t="s">
         <v>313</v>
       </c>
@@ -5460,7 +5453,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="133" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="2" t="s">
         <v>316</v>
       </c>
@@ -5489,7 +5482,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="134" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="2" t="s">
         <v>319</v>
       </c>
@@ -5518,7 +5511,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="135" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="2" t="s">
         <v>320</v>
       </c>
@@ -5547,7 +5540,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="136" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="2" t="s">
         <v>323</v>
       </c>
@@ -5576,7 +5569,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="137" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="2" t="s">
         <v>326</v>
       </c>
@@ -5605,7 +5598,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="138" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="2" t="s">
         <v>327</v>
       </c>
@@ -5634,7 +5627,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="139" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="2" t="s">
         <v>328</v>
       </c>
@@ -5663,7 +5656,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="140" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="2" t="s">
         <v>329</v>
       </c>
@@ -5692,7 +5685,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="141" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="2" t="s">
         <v>330</v>
       </c>
@@ -5721,7 +5714,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="142" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="2" t="s">
         <v>333</v>
       </c>
@@ -5750,7 +5743,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="143" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="2" t="s">
         <v>336</v>
       </c>
@@ -5779,7 +5772,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="144" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="2" t="s">
         <v>337</v>
       </c>
@@ -5808,7 +5801,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="145" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="2" t="s">
         <v>338</v>
       </c>
@@ -5837,7 +5830,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="146" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="2" t="s">
         <v>341</v>
       </c>
@@ -5866,7 +5859,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="147" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="2" t="s">
         <v>342</v>
       </c>
@@ -5895,7 +5888,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="148" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="2" t="s">
         <v>343</v>
       </c>
@@ -5924,7 +5917,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="149" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="2" t="s">
         <v>346</v>
       </c>
@@ -5953,7 +5946,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="150" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="2" t="s">
         <v>347</v>
       </c>
@@ -5982,7 +5975,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="151" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="2" t="s">
         <v>348</v>
       </c>
@@ -6011,7 +6004,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="152" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="2" t="s">
         <v>349</v>
       </c>
@@ -6040,7 +6033,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="153" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="2" t="s">
         <v>352</v>
       </c>
@@ -6069,7 +6062,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="154" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="2" t="s">
         <v>353</v>
       </c>
@@ -6098,7 +6091,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="155" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="2" t="s">
         <v>356</v>
       </c>
@@ -6127,7 +6120,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="156" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="2" t="s">
         <v>357</v>
       </c>
@@ -6156,7 +6149,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="157" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="2" t="s">
         <v>358</v>
       </c>
@@ -6185,7 +6178,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="158" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="2" t="s">
         <v>359</v>
       </c>
@@ -6214,7 +6207,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="159" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="2" t="s">
         <v>360</v>
       </c>
@@ -6243,7 +6236,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="160" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="2" t="s">
         <v>361</v>
       </c>
@@ -6272,7 +6265,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="161" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="2" t="s">
         <v>362</v>
       </c>
@@ -6301,7 +6294,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="162" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="2" t="s">
         <v>363</v>
       </c>
@@ -6330,7 +6323,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="163" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="2" t="s">
         <v>364</v>
       </c>
@@ -6359,7 +6352,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="164" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="2" t="s">
         <v>365</v>
       </c>
@@ -6388,7 +6381,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="165" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="2" t="s">
         <v>366</v>
       </c>
@@ -6417,7 +6410,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="166" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="2" t="s">
         <v>367</v>
       </c>
@@ -6446,7 +6439,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="167" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="2" t="s">
         <v>368</v>
       </c>
@@ -6475,7 +6468,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="168" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="2" t="s">
         <v>369</v>
       </c>
@@ -6504,7 +6497,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="169" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="2" t="s">
         <v>370</v>
       </c>
@@ -6533,7 +6526,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="170" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="2" t="s">
         <v>371</v>
       </c>
@@ -6562,7 +6555,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="171" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="2" t="s">
         <v>372</v>
       </c>
@@ -6591,7 +6584,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="172" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="2" t="s">
         <v>373</v>
       </c>
@@ -6620,7 +6613,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="173" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="2" t="s">
         <v>374</v>
       </c>
@@ -6649,7 +6642,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="174" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="2" t="s">
         <v>375</v>
       </c>
@@ -6678,7 +6671,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="175" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="2" t="s">
         <v>376</v>
       </c>
@@ -6707,7 +6700,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="176" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="2" t="s">
         <v>377</v>
       </c>
@@ -6736,7 +6729,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="177" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="2" t="s">
         <v>379</v>
       </c>
@@ -6765,7 +6758,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="178" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="3" t="s">
         <v>380</v>
       </c>
@@ -6794,7 +6787,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="179" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="3" t="s">
         <v>387</v>
       </c>
@@ -6823,7 +6816,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="180" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="3" t="s">
         <v>388</v>
       </c>
@@ -6852,7 +6845,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="181" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="3" t="s">
         <v>389</v>
       </c>
@@ -6881,7 +6874,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="182" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="3" t="s">
         <v>390</v>
       </c>
@@ -6910,7 +6903,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="183" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="3" t="s">
         <v>391</v>
       </c>
@@ -6939,7 +6932,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="184" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="3" t="s">
         <v>392</v>
       </c>
@@ -6968,7 +6961,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="185" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="3" t="s">
         <v>393</v>
       </c>
@@ -6997,7 +6990,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="186" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="2" t="s">
         <v>394</v>
       </c>
@@ -7026,7 +7019,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="187" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="2" t="s">
         <v>400</v>
       </c>
@@ -7055,7 +7048,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="188" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="2" t="s">
         <v>405</v>
       </c>
@@ -7084,7 +7077,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="189" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="2" t="s">
         <v>409</v>
       </c>
@@ -7113,7 +7106,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="190" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="2" t="s">
         <v>410</v>
       </c>
@@ -7142,7 +7135,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="191" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="2" t="s">
         <v>415</v>
       </c>
@@ -7171,7 +7164,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="192" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="2" t="s">
         <v>420</v>
       </c>
@@ -7200,642 +7193,642 @@
         <v>252</v>
       </c>
     </row>
-    <row r="193" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A193" s="7" t="s">
+    <row r="193" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A193" s="6" t="s">
         <v>424</v>
       </c>
-      <c r="B193" s="7" t="s">
+      <c r="B193" s="6" t="s">
         <v>425</v>
       </c>
-      <c r="C193" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D193" s="7" t="s">
+      <c r="C193" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D193" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E193" s="6" t="s">
+        <v>396</v>
+      </c>
+      <c r="F193" s="6" t="s">
         <v>426</v>
       </c>
-      <c r="E193" s="7" t="s">
+      <c r="G193" s="6" t="s">
         <v>427</v>
       </c>
-      <c r="F193" s="7" t="s">
+      <c r="H193" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I193" s="6" t="s">
         <v>428</v>
-      </c>
-      <c r="G193" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H193" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="I193" s="7" t="s">
-        <v>429</v>
       </c>
     </row>
     <row r="194" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="B194" s="2" t="s">
         <v>430</v>
       </c>
-      <c r="B194" s="2" t="s">
+      <c r="C194" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D194" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E194" s="2" t="s">
         <v>431</v>
       </c>
-      <c r="C194" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D194" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E194" s="2" t="s">
+      <c r="F194" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="G194" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H194" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I194" s="2" t="s">
         <v>432</v>
-      </c>
-      <c r="F194" s="2" t="s">
-        <v>431</v>
-      </c>
-      <c r="G194" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H194" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I194" s="2" t="s">
-        <v>433</v>
       </c>
     </row>
     <row r="195" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="2" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B195" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="C195" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D195" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E195" s="2" t="s">
         <v>431</v>
       </c>
-      <c r="C195" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D195" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E195" s="2" t="s">
+      <c r="F195" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="G195" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H195" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I195" s="2" t="s">
         <v>432</v>
-      </c>
-      <c r="F195" s="2" t="s">
-        <v>431</v>
-      </c>
-      <c r="G195" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H195" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I195" s="2" t="s">
-        <v>433</v>
       </c>
     </row>
     <row r="196" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="2" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B196" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="C196" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D196" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E196" s="2" t="s">
         <v>431</v>
       </c>
-      <c r="C196" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D196" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E196" s="2" t="s">
+      <c r="F196" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="G196" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H196" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I196" s="2" t="s">
         <v>432</v>
-      </c>
-      <c r="F196" s="2" t="s">
-        <v>431</v>
-      </c>
-      <c r="G196" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H196" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I196" s="2" t="s">
-        <v>433</v>
       </c>
     </row>
     <row r="197" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="2" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B197" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="C197" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D197" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E197" s="2" t="s">
         <v>431</v>
       </c>
-      <c r="C197" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D197" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E197" s="2" t="s">
+      <c r="F197" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="G197" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H197" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I197" s="2" t="s">
         <v>432</v>
-      </c>
-      <c r="F197" s="2" t="s">
-        <v>431</v>
-      </c>
-      <c r="G197" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H197" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I197" s="2" t="s">
-        <v>433</v>
       </c>
     </row>
     <row r="198" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="2" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B198" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="C198" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D198" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E198" s="2" t="s">
         <v>431</v>
       </c>
-      <c r="C198" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D198" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E198" s="2" t="s">
+      <c r="F198" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="G198" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H198" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I198" s="2" t="s">
         <v>432</v>
-      </c>
-      <c r="F198" s="2" t="s">
-        <v>431</v>
-      </c>
-      <c r="G198" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H198" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I198" s="2" t="s">
-        <v>433</v>
       </c>
     </row>
     <row r="199" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="2" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B199" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="C199" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D199" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E199" s="2" t="s">
         <v>431</v>
       </c>
-      <c r="C199" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D199" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E199" s="2" t="s">
+      <c r="F199" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="G199" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H199" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I199" s="2" t="s">
         <v>432</v>
-      </c>
-      <c r="F199" s="2" t="s">
-        <v>431</v>
-      </c>
-      <c r="G199" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H199" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I199" s="2" t="s">
-        <v>433</v>
       </c>
     </row>
     <row r="200" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="2" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B200" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="C200" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D200" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E200" s="2" t="s">
         <v>431</v>
       </c>
-      <c r="C200" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D200" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E200" s="2" t="s">
+      <c r="F200" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="G200" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H200" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I200" s="2" t="s">
         <v>432</v>
-      </c>
-      <c r="F200" s="2" t="s">
-        <v>431</v>
-      </c>
-      <c r="G200" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H200" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I200" s="2" t="s">
-        <v>433</v>
       </c>
     </row>
     <row r="201" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B201" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="C201" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D201" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E201" s="2" t="s">
         <v>431</v>
       </c>
-      <c r="C201" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D201" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E201" s="2" t="s">
+      <c r="F201" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="G201" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H201" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I201" s="2" t="s">
         <v>432</v>
-      </c>
-      <c r="F201" s="2" t="s">
-        <v>431</v>
-      </c>
-      <c r="G201" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H201" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I201" s="2" t="s">
-        <v>433</v>
       </c>
     </row>
     <row r="202" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="2" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B202" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="C202" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D202" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E202" s="2" t="s">
         <v>431</v>
       </c>
-      <c r="C202" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D202" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E202" s="2" t="s">
+      <c r="F202" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="G202" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H202" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I202" s="2" t="s">
         <v>432</v>
-      </c>
-      <c r="F202" s="2" t="s">
-        <v>431</v>
-      </c>
-      <c r="G202" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H202" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I202" s="2" t="s">
-        <v>433</v>
       </c>
     </row>
     <row r="203" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="B203" s="2" t="s">
         <v>442</v>
       </c>
-      <c r="B203" s="2" t="s">
+      <c r="C203" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D203" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E203" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F203" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G203" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H203" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I203" s="2" t="s">
         <v>443</v>
-      </c>
-      <c r="C203" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D203" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E203" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F203" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G203" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H203" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I203" s="2" t="s">
-        <v>444</v>
       </c>
     </row>
     <row r="204" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B204" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="C204" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D204" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E204" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F204" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G204" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H204" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I204" s="2" t="s">
         <v>443</v>
-      </c>
-      <c r="C204" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D204" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E204" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F204" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G204" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H204" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I204" s="2" t="s">
-        <v>444</v>
       </c>
     </row>
     <row r="205" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="2" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B205" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="C205" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D205" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E205" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F205" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G205" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H205" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I205" s="2" t="s">
         <v>443</v>
-      </c>
-      <c r="C205" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D205" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E205" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F205" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G205" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H205" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I205" s="2" t="s">
-        <v>444</v>
       </c>
     </row>
     <row r="206" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="2" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B206" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="C206" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D206" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E206" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F206" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G206" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H206" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I206" s="2" t="s">
         <v>443</v>
-      </c>
-      <c r="C206" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D206" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E206" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F206" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G206" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H206" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I206" s="2" t="s">
-        <v>444</v>
       </c>
     </row>
     <row r="207" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="2" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B207" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="C207" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D207" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E207" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F207" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G207" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H207" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I207" s="2" t="s">
         <v>443</v>
-      </c>
-      <c r="C207" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D207" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E207" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F207" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G207" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H207" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I207" s="2" t="s">
-        <v>444</v>
       </c>
     </row>
     <row r="208" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="B208" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="C208" s="2" t="s">
         <v>449</v>
       </c>
-      <c r="B208" s="2" t="s">
+      <c r="D208" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E208" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F208" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G208" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H208" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I208" s="2" t="s">
         <v>443</v>
-      </c>
-      <c r="C208" s="2" t="s">
-        <v>450</v>
-      </c>
-      <c r="D208" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E208" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F208" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G208" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H208" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I208" s="2" t="s">
-        <v>444</v>
       </c>
     </row>
     <row r="209" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="B209" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="C209" s="2" t="s">
         <v>451</v>
       </c>
-      <c r="B209" s="2" t="s">
+      <c r="D209" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E209" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F209" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G209" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H209" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I209" s="2" t="s">
         <v>443</v>
-      </c>
-      <c r="C209" s="2" t="s">
-        <v>452</v>
-      </c>
-      <c r="D209" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E209" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F209" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G209" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H209" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I209" s="2" t="s">
-        <v>444</v>
       </c>
     </row>
     <row r="210" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="2" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B210" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="C210" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="D210" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E210" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F210" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G210" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H210" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I210" s="2" t="s">
         <v>443</v>
-      </c>
-      <c r="C210" s="2" t="s">
-        <v>452</v>
-      </c>
-      <c r="D210" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E210" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F210" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G210" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H210" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I210" s="2" t="s">
-        <v>444</v>
       </c>
     </row>
     <row r="211" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="2" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B211" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="C211" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="D211" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E211" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F211" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G211" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H211" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I211" s="2" t="s">
         <v>443</v>
-      </c>
-      <c r="C211" s="2" t="s">
-        <v>452</v>
-      </c>
-      <c r="D211" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E211" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F211" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G211" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H211" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I211" s="2" t="s">
-        <v>444</v>
       </c>
     </row>
     <row r="212" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="2" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B212" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="C212" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="D212" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E212" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F212" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G212" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H212" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I212" s="2" t="s">
         <v>443</v>
-      </c>
-      <c r="C212" s="2" t="s">
-        <v>452</v>
-      </c>
-      <c r="D212" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E212" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F212" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G212" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H212" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I212" s="2" t="s">
-        <v>444</v>
       </c>
     </row>
     <row r="213" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="2" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B213" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="C213" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="D213" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E213" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F213" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G213" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H213" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I213" s="2" t="s">
         <v>443</v>
-      </c>
-      <c r="C213" s="2" t="s">
-        <v>452</v>
-      </c>
-      <c r="D213" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E213" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F213" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G213" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H213" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I213" s="2" t="s">
-        <v>444</v>
       </c>
     </row>
     <row r="214" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="2" t="s">
+        <v>456</v>
+      </c>
+      <c r="B214" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="C214" s="2" t="s">
         <v>457</v>
       </c>
-      <c r="B214" s="2" t="s">
+      <c r="D214" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E214" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F214" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G214" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H214" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I214" s="2" t="s">
         <v>443</v>
-      </c>
-      <c r="C214" s="2" t="s">
-        <v>458</v>
-      </c>
-      <c r="D214" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E214" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F214" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G214" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H214" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I214" s="2" t="s">
-        <v>444</v>
       </c>
     </row>
     <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>